<commit_message>
Code to insert card list effective 2014-10-28.
</commit_message>
<xml_diff>
--- a/cardshifter-database/TCG card list 10-28-14.xlsx
+++ b/cardshifter-database/TCG card list 10-28-14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24700" windowHeight="15420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24700" windowHeight="15440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="155">
   <si>
     <t>id</t>
   </si>
@@ -86,54 +86,6 @@
     <t xml:space="preserve">Heat Shielding </t>
   </si>
   <si>
-    <t>Balance-3</t>
-  </si>
-  <si>
-    <t>BalanceMech-1</t>
-  </si>
-  <si>
-    <t>AttackMech-1</t>
-  </si>
-  <si>
-    <t>DefenseMech-1</t>
-  </si>
-  <si>
-    <t>BalanceMech-2</t>
-  </si>
-  <si>
-    <t>ScrapMech</t>
-  </si>
-  <si>
-    <t>DefenseMech-2</t>
-  </si>
-  <si>
-    <t>AttackMech-2</t>
-  </si>
-  <si>
-    <t>DefenseMech-3</t>
-  </si>
-  <si>
-    <t>Street Punk</t>
-  </si>
-  <si>
-    <t>Street Thug</t>
-  </si>
-  <si>
-    <t>Fighter</t>
-  </si>
-  <si>
-    <t>Retired Soldier</t>
-  </si>
-  <si>
-    <t>Sniper</t>
-  </si>
-  <si>
-    <t>Bodyguard</t>
-  </si>
-  <si>
-    <t>Elite Commando</t>
-  </si>
-  <si>
     <t>Body Armor</t>
   </si>
   <si>
@@ -158,9 +110,6 @@
     <t>Artificial Intelligence Implants</t>
   </si>
   <si>
-    <t>Gang Leader</t>
-  </si>
-  <si>
     <t>Spell</t>
   </si>
   <si>
@@ -251,9 +200,6 @@
     <t>flavor_text</t>
   </si>
   <si>
-    <t>generic_name</t>
-  </si>
-  <si>
     <t>Spareparts</t>
   </si>
   <si>
@@ -281,12 +227,6 @@
     <t>Supply Mech</t>
   </si>
   <si>
-    <t>DefenseMech4</t>
-  </si>
-  <si>
-    <t>RushMech-1</t>
-  </si>
-  <si>
     <t>Rush. No cast sickness.</t>
   </si>
   <si>
@@ -329,9 +269,6 @@
     <t>Uses the legs of other bots to enhance its own speed.</t>
   </si>
   <si>
-    <t>RushMech-2</t>
-  </si>
-  <si>
     <t>Bodyman</t>
   </si>
   <si>
@@ -549,6 +486,9 @@
   </si>
   <si>
     <t>Upgrade a Mech +3/+3 for a cost in Scrap.</t>
+  </si>
+  <si>
+    <t>version</t>
   </si>
 </sst>
 </file>
@@ -699,8 +639,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -830,15 +780,25 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1134,23 +1094,21 @@
   <dimension ref="A1:Y57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="N48" sqref="N48"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="2"/>
-    <col min="2" max="2" width="28.6640625" style="6" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="34.5" style="6" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="39" style="14" customWidth="1"/>
-    <col min="6" max="6" width="39" style="14" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="34.5" style="6" customWidth="1"/>
+    <col min="5" max="6" width="39" style="14" customWidth="1"/>
     <col min="7" max="7" width="45" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45" style="37" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="45" style="37" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" style="2"/>
-    <col min="10" max="10" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="2" customWidth="1"/>
     <col min="11" max="11" width="5.83203125" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.5" style="11" bestFit="1" customWidth="1"/>
@@ -1173,7 +1131,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
@@ -1182,16 +1140,16 @@
         <v>1</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="H2" s="36" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>2</v>
@@ -1221,40 +1179,41 @@
         <v>9</v>
       </c>
       <c r="R2" s="23" t="str">
-        <f>"START TRANSACTION; INSERT INTO CARDS("&amp;D2&amp;","&amp;F2&amp;","&amp;H2&amp;","&amp;J2&amp;","&amp;K2&amp;","&amp;L2&amp;","&amp;M2&amp;","&amp;N2&amp;","&amp;O2&amp;","&amp;P2&amp;","&amp;Q2&amp;") VALUES"</f>
-        <v>START TRANSACTION; INSERT INTO CARDS(name,flavor text,effect_description,type,attack,health,mana_cost,scrap_value,scrap_cost,sickness,attack_available) VALUES</v>
+        <f>"START TRANSACTION; SET SEARCH_PATH TO cardshifter_stats; INSERT INTO card("&amp;B2&amp;","&amp;D2&amp;","&amp;F2&amp;","&amp;H2&amp;","&amp;J2&amp;","&amp;K2&amp;","&amp;L2&amp;","&amp;P2&amp;","&amp;Q2&amp;") VALUES"</f>
+        <v>START TRANSACTION; SET SEARCH_PATH TO cardshifter_stats; INSERT INTO card(version,name,flavor text,effect_description,type,attack,health,sickness,attack_available) VALUES</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="30" customHeight="1">
-      <c r="B3" s="6" t="s">
-        <v>25</v>
+      <c r="B3" s="6">
+        <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="D3" s="6" t="str">
-        <f>"'"&amp;C3&amp;"'"</f>
-        <v>'Spareparts'</v>
+        <f>"$$"&amp;C3&amp;"$$"</f>
+        <v>$$Spareparts$$</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="F3" s="14" t="str">
-        <f>"'"&amp;E3&amp;"'"</f>
-        <v>'Cobbled together from whatever was lying around at the time.'</v>
+        <f>"$$"&amp;E3&amp;"$$"</f>
+        <v>$$Cobbled together from whatever was lying around at the time.$$</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="37" t="s">
-        <v>13</v>
+      <c r="H3" s="37" t="str">
+        <f>"$$"&amp;G3&amp;"$$"</f>
+        <v>$$null$$</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f>"'"&amp;I4&amp;"'"</f>
-        <v>'Mech'</v>
+        <f>"$$"&amp;I4&amp;"$$"</f>
+        <v>$$Mech$$</v>
       </c>
       <c r="K3" s="11">
         <v>0</v>
@@ -1277,42 +1236,42 @@
       <c r="Q3" s="50">
         <v>1</v>
       </c>
-      <c r="R3" s="11" t="str">
-        <f>"("&amp;D3&amp;","&amp;F3&amp;","&amp;H3&amp;","&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;","&amp;M3&amp;","&amp;N3&amp;","&amp;O3&amp;","&amp;P3&amp;","&amp;Q3&amp;"),"</f>
-        <v>('Spareparts','Cobbled together from whatever was lying around at the time.',null,'Mech',0,1,0,3,null,1,1),</v>
+      <c r="R3" s="23" t="str">
+        <f>"("&amp;B3&amp;","&amp;D3&amp;","&amp;F3&amp;","&amp;H3&amp;","&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;","&amp;P3&amp;","&amp;Q3&amp;"),"</f>
+        <v>(1,$$Spareparts$$,$$Cobbled together from whatever was lying around at the time.$$,$$null$$,$$Mech$$,0,1,1,1),</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="30" customHeight="1">
-      <c r="B4" s="6" t="s">
-        <v>21</v>
+      <c r="B4" s="6">
+        <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D4" s="6" t="str">
-        <f t="shared" ref="D4:D56" si="0">"'"&amp;C4&amp;"'"</f>
-        <v>'Gyrodroid'</v>
+        <f t="shared" ref="D4:D56" si="0">"$$"&amp;C4&amp;"$$"</f>
+        <v>$$Gyrodroid$$</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="F4" s="14" t="str">
-        <f t="shared" ref="F4:F56" si="1">"'"&amp;E4&amp;"'"</f>
-        <v>'A flying, spherical droid that shoots weak laser beams at nearby targets.'</v>
+        <f t="shared" ref="F4:F56" si="1">"$$"&amp;E4&amp;"$$"</f>
+        <v>$$A flying, spherical droid that shoots weak laser beams at nearby targets.$$</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="H4" s="37" t="str">
-        <f>"'"&amp;G4&amp;"'"</f>
-        <v>'Ranged. Suffers no damage when attacking.'</v>
+        <f>"$$"&amp;G4&amp;"$$"</f>
+        <v>$$Ranged. Suffers no damage when attacking.$$</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="2" t="str">
-        <f t="shared" ref="J4:J56" si="2">"'"&amp;I5&amp;"'"</f>
-        <v>'Mech'</v>
+        <f t="shared" ref="J4:J56" si="2">"$$"&amp;I5&amp;"$$"</f>
+        <v>$$Mech$$</v>
       </c>
       <c r="K4" s="11">
         <v>1</v>
@@ -1335,41 +1294,42 @@
       <c r="Q4" s="50">
         <v>1</v>
       </c>
-      <c r="R4" s="11" t="str">
-        <f t="shared" ref="R4:R55" si="3">"("&amp;D4&amp;","&amp;F4&amp;","&amp;H4&amp;","&amp;J4&amp;","&amp;K4&amp;","&amp;L4&amp;","&amp;M4&amp;","&amp;N4&amp;","&amp;O4&amp;","&amp;P4&amp;","&amp;Q4&amp;"),"</f>
-        <v>('Gyrodroid','A flying, spherical droid that shoots weak laser beams at nearby targets.','Ranged. Suffers no damage when attacking.','Mech',1,1,1,1,null,1,1),</v>
+      <c r="R4" s="23" t="str">
+        <f t="shared" ref="R4:R55" si="3">"("&amp;B4&amp;",$$"&amp;C4&amp;"$$,$$"&amp;E4&amp;"$$,$$"&amp;G4&amp;"$$,$$"&amp;I4&amp;"$$,"&amp;K4&amp;","&amp;L4&amp;","&amp;P4&amp;","&amp;Q4&amp;"),"</f>
+        <v>(1,$$Gyrodroid$$,$$A flying, spherical droid that shoots weak laser beams at nearby targets.$$,$$Ranged. Suffers no damage when attacking.$$,$$Mech$$,1,1,1,1),</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="30" customHeight="1">
-      <c r="B5" s="6" t="s">
-        <v>22</v>
+      <c r="B5" s="6">
+        <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'The Chopper'</v>
+        <v>$$The Chopper$$</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="F5" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'Looks like a flying circular blade with a sphere in the middle.'</v>
+        <v>$$Looks like a flying circular blade with a sphere in the middle.$$</v>
       </c>
       <c r="G5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="37" t="s">
-        <v>13</v>
+      <c r="H5" s="37" t="str">
+        <f t="shared" ref="H5:H56" si="4">"$$"&amp;G5&amp;"$$"</f>
+        <v>$$null$$</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Mech'</v>
+        <v>$$Mech$$</v>
       </c>
       <c r="K5" s="11">
         <v>2</v>
@@ -1392,41 +1352,42 @@
       <c r="Q5" s="50">
         <v>1</v>
       </c>
-      <c r="R5" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('The Chopper','Looks like a flying circular blade with a sphere in the middle.',null,'Mech',2,1,2,1,null,1,1),</v>
+      <c r="R5" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$The Chopper$$,$$Looks like a flying circular blade with a sphere in the middle.$$,$$null$$,$$Mech$$,2,1,1,1),</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="30" customHeight="1">
-      <c r="B6" s="6" t="s">
-        <v>23</v>
+      <c r="B6" s="6">
+        <v>1</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Shieldmech'</v>
+        <v>$$Shieldmech$$</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="F6" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'A small, flying shield generator droid.'</v>
+        <v>$$A small, flying shield generator droid.$$</v>
       </c>
       <c r="G6" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="37" t="s">
-        <v>13</v>
+      <c r="H6" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Mech'</v>
+        <v>$$Mech$$</v>
       </c>
       <c r="K6" s="11">
         <v>1</v>
@@ -1449,41 +1410,42 @@
       <c r="Q6" s="50">
         <v>1</v>
       </c>
-      <c r="R6" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Shieldmech','A small, flying shield generator droid.',null,'Mech',1,2,2,1,null,1,1),</v>
+      <c r="R6" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Shieldmech$$,$$A small, flying shield generator droid.$$,$$null$$,$$Mech$$,1,2,1,1),</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="30" customHeight="1">
-      <c r="B7" s="6" t="s">
-        <v>24</v>
+      <c r="B7" s="6">
+        <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Humadroid'</v>
+        <v>$$Humadroid$$</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="F7" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'You might mistake it for a human, but it won’t mistake you for a mech.'</v>
+        <v>$$You might mistake it for a human, but it won’t mistake you for a mech.$$</v>
       </c>
       <c r="G7" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="37" t="s">
-        <v>13</v>
+      <c r="H7" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J7" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Mech'</v>
+        <v>$$Mech$$</v>
       </c>
       <c r="K7" s="11">
         <v>3</v>
@@ -1506,42 +1468,42 @@
       <c r="Q7" s="50">
         <v>1</v>
       </c>
-      <c r="R7" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Humadroid','You might mistake it for a human, but it won’t mistake you for a mech.',null,'Mech',3,3,3,2,null,1,1),</v>
+      <c r="R7" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Humadroid$$,$$You might mistake it for a human, but it won’t mistake you for a mech.$$,$$null$$,$$Mech$$,3,3,1,1),</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="30" customHeight="1">
-      <c r="B8" s="6" t="s">
-        <v>27</v>
+      <c r="B8" s="6">
+        <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Assasinatrix'</v>
+        <v>$$Assasinatrix$$</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="F8" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'Humanoid in form, except for two massive cannons in place of arms.'</v>
+        <v>$$Humanoid in form, except for two massive cannons in place of arms.$$</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="H8" s="37" t="str">
-        <f t="shared" ref="H8:H56" si="4">"'"&amp;G8&amp;"'"</f>
-        <v>'Ranged. Suffers no damage when attacking.'</v>
+        <f t="shared" si="4"/>
+        <v>$$Ranged. Suffers no damage when attacking.$$</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J8" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Mech'</v>
+        <v>$$Mech$$</v>
       </c>
       <c r="K8" s="11">
         <v>4</v>
@@ -1564,41 +1526,42 @@
       <c r="Q8" s="50">
         <v>1</v>
       </c>
-      <c r="R8" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Assasinatrix','Humanoid in form, except for two massive cannons in place of arms.','Ranged. Suffers no damage when attacking.','Mech',4,2,3,2,null,1,1),</v>
+      <c r="R8" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Assasinatrix$$,$$Humanoid in form, except for two massive cannons in place of arms.$$,$$Ranged. Suffers no damage when attacking.$$,$$Mech$$,4,2,1,1),</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="30" customHeight="1">
-      <c r="B9" s="6" t="s">
-        <v>26</v>
+      <c r="B9" s="6">
+        <v>1</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Fortimech'</v>
+        <v>$$Fortimech$$</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="F9" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'About the only place that a hume is safe during a firefight is inside one of these.'</v>
+        <v>$$About the only place that a hume is safe during a firefight is inside one of these.$$</v>
       </c>
       <c r="G9" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="37" t="s">
-        <v>13</v>
+      <c r="H9" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J9" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Mech'</v>
+        <v>$$Mech$$</v>
       </c>
       <c r="K9" s="11">
         <v>2</v>
@@ -1621,42 +1584,42 @@
       <c r="Q9" s="50">
         <v>1</v>
       </c>
-      <c r="R9" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Fortimech','About the only place that a hume is safe during a firefight is inside one of these.',null,'Mech',2,4,3,2,null,1,1),</v>
+      <c r="R9" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Fortimech$$,$$About the only place that a hume is safe during a firefight is inside one of these.$$,$$null$$,$$Mech$$,2,4,1,1),</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="19" customFormat="1" ht="30" customHeight="1">
-      <c r="B10" s="20" t="s">
-        <v>86</v>
+      <c r="B10" s="20">
+        <v>1</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="D10" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>'Scout Mech'</v>
+        <v>$$Scout Mech$$</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F10" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>'The fastest mech on two legs. You don’t want to see the ones with four.'</v>
+        <v>$$The fastest mech on two legs. You don’t want to see the ones with four.$$</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="H10" s="38" t="str">
         <f t="shared" si="4"/>
-        <v>'Rush. No cast sickness.'</v>
+        <v>$$Rush. No cast sickness.$$</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>10</v>
       </c>
       <c r="J10" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>'Mech'</v>
+        <v>$$Mech$$</v>
       </c>
       <c r="K10" s="22">
         <v>5</v>
@@ -1679,42 +1642,42 @@
       <c r="Q10" s="52">
         <v>1</v>
       </c>
-      <c r="R10" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Scout Mech','The fastest mech on two legs. You don’t want to see the ones with four.','Rush. No cast sickness.','Mech',5,1,3,2,null,null,1),</v>
+      <c r="R10" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Scout Mech$$,$$The fastest mech on two legs. You don’t want to see the ones with four.$$,$$Rush. No cast sickness.$$,$$Mech$$,5,1,null,1),</v>
       </c>
     </row>
     <row r="11" spans="1:18" s="19" customFormat="1" ht="30" customHeight="1">
-      <c r="B11" s="20" t="s">
-        <v>85</v>
+      <c r="B11" s="20">
+        <v>1</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="D11" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>'Supply Mech'</v>
+        <v>$$Supply Mech$$</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="F11" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>'Worth more than its weight in scrap, and it is pretty heavy.'</v>
+        <v>$$Worth more than its weight in scrap, and it is pretty heavy.$$</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="H11" s="38" t="str">
         <f t="shared" si="4"/>
-        <v>'Cannot attack.'</v>
+        <v>$$Cannot attack.$$</v>
       </c>
       <c r="I11" s="19" t="s">
         <v>10</v>
       </c>
       <c r="J11" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>'Mech'</v>
+        <v>$$Mech$$</v>
       </c>
       <c r="K11" s="22">
         <v>0</v>
@@ -1737,42 +1700,42 @@
       <c r="Q11" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Supply Mech','Worth more than its weight in scrap, and it is pretty heavy.','Cannot attack.','Mech',0,5,3,3,null,1,null),</v>
+      <c r="R11" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Supply Mech$$,$$Worth more than its weight in scrap, and it is pretty heavy.$$,$$Cannot attack.$$,$$Mech$$,0,5,1,null),</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="30" customHeight="1">
-      <c r="B12" s="20" t="s">
-        <v>101</v>
+      <c r="B12" s="20">
+        <v>1</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Modleg Ambusher'</v>
+        <v>$$Modleg Ambusher$$</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F12" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'Uses the legs of other bots to enhance its own speed.'</v>
+        <v>$$Uses the legs of other bots to enhance its own speed.$$</v>
       </c>
       <c r="G12" s="47" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="H12" s="47" t="str">
         <f t="shared" si="4"/>
-        <v>'Rush. No cast sickness.'</v>
+        <v>$$Rush. No cast sickness.$$</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J12" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Mech'</v>
+        <v>$$Mech$$</v>
       </c>
       <c r="K12" s="23">
         <v>5</v>
@@ -1795,41 +1758,42 @@
       <c r="Q12" s="50">
         <v>1</v>
       </c>
-      <c r="R12" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Modleg Ambusher','Uses the legs of other bots to enhance its own speed.','Rush. No cast sickness.','Mech',5,3,5,3,null,null,1),</v>
+      <c r="R12" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Modleg Ambusher$$,$$Uses the legs of other bots to enhance its own speed.$$,$$Rush. No cast sickness.$$,$$Mech$$,5,3,null,1),</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="30" customHeight="1">
-      <c r="B13" s="6" t="s">
-        <v>28</v>
+      <c r="B13" s="6">
+        <v>1</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="D13" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>'Heavy Mech'</v>
+        <v>$$Heavy Mech$$</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="F13" s="49" t="str">
         <f t="shared" si="1"/>
-        <v>'The bigger they are, the harder they fall. Eventually.'</v>
+        <v>$$The bigger they are, the harder they fall. Eventually.$$</v>
       </c>
       <c r="G13" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="37" t="s">
-        <v>13</v>
+      <c r="H13" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J13" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Mech'</v>
+        <v>$$Mech$$</v>
       </c>
       <c r="K13" s="23">
         <v>3</v>
@@ -1852,41 +1816,42 @@
       <c r="Q13" s="50">
         <v>1</v>
       </c>
-      <c r="R13" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Heavy Mech','The bigger they are, the harder they fall. Eventually.',null,'Mech',3,6,5,3,null,1,1),</v>
+      <c r="R13" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Heavy Mech$$,$$The bigger they are, the harder they fall. Eventually.$$,$$null$$,$$Mech$$,3,6,1,1),</v>
       </c>
     </row>
     <row r="14" spans="1:18" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="B14" s="7" t="s">
-        <v>20</v>
+      <c r="B14" s="7">
+        <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="D14" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>'Waste Runner'</v>
+        <v>$$Waste Runner$$</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="F14" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>'Armored and armed with superior arms.'</v>
+        <v>$$Armored and armed with superior arms.$$</v>
       </c>
       <c r="G14" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="39" t="s">
-        <v>13</v>
+      <c r="H14" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J14" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>'Hume'</v>
+        <v>$$Hume$$</v>
       </c>
       <c r="K14" s="26">
         <v>4</v>
@@ -1909,42 +1874,42 @@
       <c r="Q14" s="53">
         <v>1</v>
       </c>
-      <c r="R14" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Waste Runner','Armored and armed with superior arms.',null,'Hume',4,4,5,3,null,1,1),</v>
+      <c r="R14" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Waste Runner$$,$$Armored and armed with superior arms.$$,$$null$$,$$Mech$$,4,4,1,1),</v>
       </c>
     </row>
     <row r="15" spans="1:18" s="30" customFormat="1" ht="30" customHeight="1">
-      <c r="B15" s="28" t="s">
-        <v>13</v>
+      <c r="B15" s="28">
+        <v>1</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D15" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>'Lost Soul'</v>
+        <v>$$Lost Soul$$</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="F15" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>'Echo of a powerful jacker that wanders the computerized wastes.'</v>
+        <v>$$Echo of a powerful jacker that wanders the computerized wastes.$$</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="H15" s="40" t="str">
         <f t="shared" si="4"/>
-        <v>'Steal 1 enemy Mech from the playing field.'</v>
+        <v>$$Steal 1 enemy Mech from the playing field.$$</v>
       </c>
       <c r="I15" s="30" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="J15" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>'Hume'</v>
+        <v>$$Hume$$</v>
       </c>
       <c r="K15" s="29">
         <v>2</v>
@@ -1967,42 +1932,42 @@
       <c r="Q15" s="52">
         <v>1</v>
       </c>
-      <c r="R15" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Lost Soul','Echo of a powerful jacker that wanders the computerized wastes.','Steal 1 enemy Mech from the playing field.','Hume',2,5,3,null,null,null,1),</v>
+      <c r="R15" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Lost Soul$$,$$Echo of a powerful jacker that wanders the computerized wastes.$$,$$Steal 1 enemy Mech from the playing field.$$,$$Hume$$,2,5,null,1),</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="30" customFormat="1" ht="30" customHeight="1">
-      <c r="B16" s="28" t="s">
-        <v>13</v>
+      <c r="B16" s="28">
+        <v>1</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="D16" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>'Slacker Jacker'</v>
+        <v>$$Slacker Jacker$$</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="F16" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>'Spends all of his time jacked into the web.'</v>
+        <v>$$Spends all of his time jacked into the web.$$</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="H16" s="40" t="str">
         <f t="shared" si="4"/>
-        <v>'All enemy Mechs have -1/-1 while this Hume is in play.'</v>
+        <v>$$All enemy Mechs have -1/-1 while this Hume is in play.$$</v>
       </c>
       <c r="I16" s="30" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="J16" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>'Hume'</v>
+        <v>$$Hume$$</v>
       </c>
       <c r="K16" s="29">
         <v>0</v>
@@ -2025,42 +1990,42 @@
       <c r="Q16" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="R16" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Slacker Jacker','Spends all of his time jacked into the web.','All enemy Mechs have -1/-1 while this Hume is in play.','Hume',0,5,3,null,null,null,null),</v>
+      <c r="R16" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Slacker Jacker$$,$$Spends all of his time jacked into the web.$$,$$All enemy Mechs have -1/-1 while this Hume is in play.$$,$$Hume$$,0,5,null,null),</v>
       </c>
     </row>
     <row r="17" spans="1:25" s="32" customFormat="1" ht="30" customHeight="1">
-      <c r="B17" s="33" t="s">
-        <v>13</v>
+      <c r="B17" s="33">
+        <v>1</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="D17" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>'Spook'</v>
+        <v>$$Spook$$</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="F17" s="34" t="str">
         <f t="shared" si="1"/>
-        <v>'Hume that donated their human body to have their consciousness uploaded to the web.'</v>
+        <v>$$Hume that donated their human body to have their consciousness uploaded to the web.$$</v>
       </c>
       <c r="G17" s="41" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="H17" s="41" t="str">
         <f t="shared" si="4"/>
-        <v>'All friendly Mechs have +1/+1 while this Hume is in play.'</v>
+        <v>$$All friendly Mechs have +1/+1 while this Hume is in play.$$</v>
       </c>
       <c r="I17" s="32" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="J17" s="32" t="str">
         <f t="shared" si="2"/>
-        <v>'Bio'</v>
+        <v>$$Bio$$</v>
       </c>
       <c r="K17" s="35">
         <v>0</v>
@@ -2083,41 +2048,42 @@
       <c r="Q17" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="R17" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Spook','Hume that donated their human body to have their consciousness uploaded to the web.','All friendly Mechs have +1/+1 while this Hume is in play.','Bio',0,5,3,null,null,null,null),</v>
+      <c r="R17" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Spook$$,$$Hume that donated their human body to have their consciousness uploaded to the web.$$,$$All friendly Mechs have +1/+1 while this Hume is in play.$$,$$Hume$$,0,5,null,null),</v>
       </c>
     </row>
     <row r="18" spans="1:25" s="30" customFormat="1" ht="30" customHeight="1">
-      <c r="B18" s="28" t="s">
-        <v>13</v>
+      <c r="B18" s="28">
+        <v>1</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="D18" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>'Conscript'</v>
+        <v>$$Conscript$$</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="F18" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>'He just signed up last week and he is very excited to fight.'</v>
+        <v>$$He just signed up last week and he is very excited to fight.$$</v>
       </c>
       <c r="G18" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="40" t="s">
-        <v>13</v>
+      <c r="H18" s="40" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I18" s="30" t="s">
         <v>11</v>
       </c>
       <c r="J18" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>'Bio'</v>
+        <v>$$Bio$$</v>
       </c>
       <c r="K18" s="29">
         <v>2</v>
@@ -2140,43 +2106,43 @@
       <c r="Q18" s="52">
         <v>1</v>
       </c>
-      <c r="R18" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Conscript','He just signed up last week and he is very excited to fight.',null,'Bio',2,2,2,null,null,1,1),</v>
+      <c r="R18" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Conscript$$,$$He just signed up last week and he is very excited to fight.$$,$$null$$,$$Bio$$,2,2,1,1),</v>
       </c>
     </row>
     <row r="19" spans="1:25" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A19" s="29"/>
-      <c r="B19" s="13" t="s">
-        <v>29</v>
+      <c r="B19" s="13">
+        <v>1</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D19" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>'Longshot'</v>
+        <v>$$Longshot$$</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="F19" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>'Eyes and reflexes augmented for maximum deadliness.'</v>
+        <v>$$Eyes and reflexes augmented for maximum deadliness.$$</v>
       </c>
       <c r="G19" s="37" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="H19" s="37" t="str">
         <f t="shared" si="4"/>
-        <v>'Ranged. Suffers no damage when attacking.'</v>
+        <v>$$Ranged. Suffers no damage when attacking.$$</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>11</v>
       </c>
       <c r="J19" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>'Bio'</v>
+        <v>$$Bio$$</v>
       </c>
       <c r="K19" s="24">
         <v>3</v>
@@ -2199,9 +2165,9 @@
       <c r="Q19" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="R19" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Longshot','Eyes and reflexes augmented for maximum deadliness.','Ranged. Suffers no damage when attacking.','Bio',3,2,3,null,null,1,null),</v>
+      <c r="R19" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Longshot$$,$$Eyes and reflexes augmented for maximum deadliness.$$,$$Ranged. Suffers no damage when attacking.$$,$$Bio$$,3,2,1,null),</v>
       </c>
       <c r="S19" s="29"/>
       <c r="T19" s="29"/>
@@ -2213,35 +2179,36 @@
     </row>
     <row r="20" spans="1:25" ht="30" customHeight="1">
       <c r="A20" s="29"/>
-      <c r="B20" s="6" t="s">
-        <v>30</v>
+      <c r="B20" s="6">
+        <v>1</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Bodyman'</v>
+        <v>$$Bodyman$$</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="F20" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'Strength augmented with mechanical musculature.'</v>
+        <v>$$Strength augmented with mechanical musculature.$$</v>
       </c>
       <c r="G20" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="37" t="s">
-        <v>13</v>
+      <c r="H20" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="J20" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Bio'</v>
+        <v>$$Bio$$</v>
       </c>
       <c r="K20" s="23">
         <v>2</v>
@@ -2264,9 +2231,9 @@
       <c r="Q20" s="50">
         <v>1</v>
       </c>
-      <c r="R20" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Bodyman','Strength augmented with mechanical musculature.',null,'Bio',2,3,4,null,null,1,1),</v>
+      <c r="R20" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Bodyman$$,$$Strength augmented with mechanical musculature.$$,$$null$$,$$Bio$$,2,3,1,1),</v>
       </c>
       <c r="S20" s="29"/>
       <c r="T20" s="29"/>
@@ -2278,35 +2245,36 @@
     </row>
     <row r="21" spans="1:25" ht="30" customHeight="1">
       <c r="A21" s="29"/>
-      <c r="B21" s="6" t="s">
-        <v>31</v>
+      <c r="B21" s="6">
+        <v>1</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Vetter'</v>
+        <v>$$Vetter$$</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="F21" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'A retired conscript with a desire to jack and make some quick creds.'</v>
+        <v>$$A retired conscript with a desire to jack and make some quick creds.$$</v>
       </c>
       <c r="G21" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="37" t="s">
-        <v>13</v>
+      <c r="H21" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="J21" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Bio'</v>
+        <v>$$Bio$$</v>
       </c>
       <c r="K21" s="23">
         <v>3</v>
@@ -2329,9 +2297,9 @@
       <c r="Q21" s="50">
         <v>1</v>
       </c>
-      <c r="R21" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Vetter','A retired conscript with a desire to jack and make some quick creds.',null,'Bio',3,3,5,null,null,1,1),</v>
+      <c r="R21" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Vetter$$,$$A retired conscript with a desire to jack and make some quick creds.$$,$$null$$,$$Bio$$,3,3,1,1),</v>
       </c>
       <c r="S21" s="29"/>
       <c r="T21" s="29"/>
@@ -2342,36 +2310,36 @@
       <c r="Y21" s="29"/>
     </row>
     <row r="22" spans="1:25" s="19" customFormat="1" ht="30" customHeight="1">
-      <c r="B22" s="20" t="s">
-        <v>13</v>
+      <c r="B22" s="20">
+        <v>1</v>
       </c>
       <c r="C22" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>$$Field Medic$$</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="D22" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>'Field Medic'</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>172</v>
-      </c>
       <c r="F22" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>'Unsung hero responsible for keeping countless troops alive.'</v>
+        <v>$$Unsung hero responsible for keeping countless troops alive.$$</v>
       </c>
       <c r="G22" s="38" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="H22" s="38" t="str">
         <f t="shared" si="4"/>
-        <v>'Heals the player for 1 health at the end of each turn'</v>
+        <v>$$Heals the player for 1 health at the end of each turn$$</v>
       </c>
       <c r="I22" s="19" t="s">
         <v>11</v>
       </c>
       <c r="J22" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>'Bio'</v>
+        <v>$$Bio$$</v>
       </c>
       <c r="K22" s="22">
         <v>1</v>
@@ -2394,42 +2362,43 @@
       <c r="Q22" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="R22" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Field Medic','Unsung hero responsible for keeping countless troops alive.','Heals the player for 1 health at the end of each turn','Bio',1,5,5,null,null,null,null),</v>
+      <c r="R22" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Field Medic$$,$$Unsung hero responsible for keeping countless troops alive.$$,$$Heals the player for 1 health at the end of each turn$$,$$Bio$$,1,5,null,null),</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="30" customHeight="1">
       <c r="A23" s="19"/>
-      <c r="B23" s="6" t="s">
-        <v>32</v>
+      <c r="B23" s="6">
+        <v>1</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Wastelander'</v>
+        <v>$$Wastelander$$</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="F23" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'Spent his life learning the lessons of the wastelands.'</v>
+        <v>$$Spent his life learning the lessons of the wastelands.$$</v>
       </c>
       <c r="G23" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="37" t="s">
-        <v>13</v>
+      <c r="H23" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="J23" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Bio'</v>
+        <v>$$Bio$$</v>
       </c>
       <c r="K23" s="23">
         <v>4</v>
@@ -2452,9 +2421,9 @@
       <c r="Q23" s="50">
         <v>1</v>
       </c>
-      <c r="R23" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Wastelander','Spent his life learning the lessons of the wastelands.',null,'Bio',4,4,6,null,null,1,1),</v>
+      <c r="R23" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Wastelander$$,$$Spent his life learning the lessons of the wastelands.$$,$$null$$,$$Bio$$,4,4,1,1),</v>
       </c>
       <c r="S23" s="19"/>
       <c r="T23" s="19"/>
@@ -2466,36 +2435,36 @@
     </row>
     <row r="24" spans="1:25" ht="30" customHeight="1">
       <c r="A24" s="19"/>
-      <c r="B24" s="6" t="s">
-        <v>33</v>
+      <c r="B24" s="6">
+        <v>1</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Commander'</v>
+        <v>$$Commander$$</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="F24" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'A professional soldier for the government.'</v>
+        <v>$$A professional soldier for the government.$$</v>
       </c>
       <c r="G24" s="47" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="H24" s="47" t="str">
         <f t="shared" si="4"/>
-        <v>'Rush. No cast sickness.'</v>
+        <v>$$Rush. No cast sickness.$$</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="J24" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Bio'</v>
+        <v>$$Bio$$</v>
       </c>
       <c r="K24" s="23">
         <v>5</v>
@@ -2518,9 +2487,9 @@
       <c r="Q24" s="50">
         <v>1</v>
       </c>
-      <c r="R24" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Commander','A professional soldier for the government.','Rush. No cast sickness.','Bio',5,3,6,null,null,1,1),</v>
+      <c r="R24" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Commander$$,$$A professional soldier for the government.$$,$$Rush. No cast sickness.$$,$$Bio$$,5,3,1,1),</v>
       </c>
       <c r="S24" s="19"/>
       <c r="T24" s="19"/>
@@ -2532,35 +2501,36 @@
     </row>
     <row r="25" spans="1:25" ht="30" customHeight="1">
       <c r="A25" s="19"/>
-      <c r="B25" s="6" t="s">
-        <v>34</v>
+      <c r="B25" s="6">
+        <v>1</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Cyberpimp'</v>
+        <v>$$Cyberpimp$$</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="F25" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'Supersized and heavily augmented.'</v>
+        <v>$$Supersized and heavily augmented.$$</v>
       </c>
       <c r="G25" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="37" t="s">
-        <v>13</v>
+      <c r="H25" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>11</v>
       </c>
       <c r="J25" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Bio'</v>
+        <v>$$Bio$$</v>
       </c>
       <c r="K25" s="23">
         <v>3</v>
@@ -2583,9 +2553,9 @@
       <c r="Q25" s="50">
         <v>1</v>
       </c>
-      <c r="R25" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Cyberpimp','Supersized and heavily augmented.',null,'Bio',3,5,6,null,null,1,1),</v>
+      <c r="R25" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Cyberpimp$$,$$Supersized and heavily augmented.$$,$$null$$,$$Bio$$,3,5,1,1),</v>
       </c>
       <c r="S25" s="19"/>
       <c r="T25" s="19"/>
@@ -2597,35 +2567,36 @@
     </row>
     <row r="26" spans="1:25" ht="30" customHeight="1">
       <c r="A26" s="19"/>
-      <c r="B26" s="6" t="s">
-        <v>44</v>
+      <c r="B26" s="6">
+        <v>1</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Cyborg'</v>
+        <v>$$Cyborg$$</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F26" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'He’s more machine than human now.'</v>
+        <v>$$He’s more machine than human now.$$</v>
       </c>
       <c r="G26" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="37" t="s">
-        <v>13</v>
+      <c r="H26" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="J26" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Bio'</v>
+        <v>$$Bio$$</v>
       </c>
       <c r="K26" s="23">
         <v>5</v>
@@ -2648,9 +2619,9 @@
       <c r="Q26" s="50">
         <v>1</v>
       </c>
-      <c r="R26" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Cyborg','He’s more machine than human now.',null,'Bio',5,5,7,null,null,1,1),</v>
+      <c r="R26" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Cyborg$$,$$He’s more machine than human now.$$,$$null$$,$$Bio$$,5,5,1,1),</v>
       </c>
       <c r="S26" s="19"/>
       <c r="T26" s="19"/>
@@ -2662,35 +2633,36 @@
     </row>
     <row r="27" spans="1:25" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="13" t="s">
-        <v>35</v>
+      <c r="B27" s="13">
+        <v>1</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="D27" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>'Web Boss'</v>
+        <v>$$Web Boss$$</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="F27" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>'Leader of a gang that primarily operates on the web.'</v>
+        <v>$$Leader of a gang that primarily operates on the web.$$</v>
       </c>
       <c r="G27" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="H27" s="42" t="s">
-        <v>13</v>
+      <c r="H27" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I27" s="9" t="s">
         <v>11</v>
       </c>
       <c r="J27" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>'Bio'</v>
+        <v>$$Bio$$</v>
       </c>
       <c r="K27" s="24">
         <v>6</v>
@@ -2713,9 +2685,9 @@
       <c r="Q27" s="50">
         <v>1</v>
       </c>
-      <c r="R27" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Web Boss','Leader of a gang that primarily operates on the web.',null,'Bio',6,6,8,null,null,1,1),</v>
+      <c r="R27" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Web Boss$$,$$Leader of a gang that primarily operates on the web.$$,$$null$$,$$Bio$$,6,6,1,1),</v>
       </c>
       <c r="S27" s="30"/>
       <c r="T27" s="30"/>
@@ -2726,36 +2698,36 @@
       <c r="Y27" s="30"/>
     </row>
     <row r="28" spans="1:25" s="32" customFormat="1" ht="30" customHeight="1">
-      <c r="B28" s="33" t="s">
-        <v>13</v>
+      <c r="B28" s="33">
+        <v>1</v>
       </c>
       <c r="C28" s="45" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="D28" s="45" t="str">
         <f t="shared" si="0"/>
-        <v>'Inside Man'</v>
+        <v>$$Inside Man$$</v>
       </c>
       <c r="E28" s="34" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="F28" s="34" t="str">
         <f t="shared" si="1"/>
-        <v>'A government official with wider web control. Usually brings friends.'</v>
+        <v>$$A government official with wider web control. Usually brings friends.$$</v>
       </c>
       <c r="G28" s="41" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="H28" s="41" t="str">
         <f t="shared" si="4"/>
-        <v>'Cannot attack. Cast 2 Bodyman minions at no cost next to this unit.'</v>
+        <v>$$Cannot attack. Cast 2 Bodyman minions at no cost next to this unit.$$</v>
       </c>
       <c r="I28" s="32" t="s">
         <v>11</v>
       </c>
       <c r="J28" s="32" t="str">
         <f t="shared" si="2"/>
-        <v>'Upgrade'</v>
+        <v>$$Upgrade$$</v>
       </c>
       <c r="K28" s="35">
         <v>2</v>
@@ -2778,42 +2750,43 @@
       <c r="Q28" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="R28" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Inside Man','A government official with wider web control. Usually brings friends.','Cannot attack. Cast 2 Bodyman minions at no cost next to this unit.','Upgrade',2,6,8,null,null,1,null),</v>
+      <c r="R28" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Inside Man$$,$$A government official with wider web control. Usually brings friends.$$,$$Cannot attack. Cast 2 Bodyman minions at no cost next to this unit.$$,$$Bio$$,2,6,1,null),</v>
       </c>
     </row>
     <row r="29" spans="1:25" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A29" s="29"/>
-      <c r="B29" s="13" t="s">
-        <v>13</v>
+      <c r="B29" s="13">
+        <v>1</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D29" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>'Bionic Arms'</v>
+        <v>$$Bionic Arms$$</v>
       </c>
       <c r="E29" s="46" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="F29" s="46" t="str">
         <f t="shared" si="1"/>
-        <v>'These arms will give strength to even the most puny individual.'</v>
+        <v>$$These arms will give strength to even the most puny individual.$$</v>
       </c>
       <c r="G29" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="42" t="s">
-        <v>13</v>
+      <c r="H29" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I29" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J29" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>'Upgrade'</v>
+        <v>$$Upgrade$$</v>
       </c>
       <c r="K29" s="24">
         <v>2</v>
@@ -2836,9 +2809,9 @@
       <c r="Q29" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R29" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Bionic Arms','These arms will give strength to even the most puny individual.',null,'Upgrade',2,0,null,null,1,null,null),</v>
+      <c r="R29" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Bionic Arms$$,$$These arms will give strength to even the most puny individual.$$,$$null$$,$$Upgrade$$,2,0,null,null),</v>
       </c>
       <c r="S29" s="29"/>
       <c r="T29" s="29"/>
@@ -2850,35 +2823,36 @@
     </row>
     <row r="30" spans="1:25" ht="30" customHeight="1">
       <c r="A30" s="29"/>
-      <c r="B30" s="6" t="s">
-        <v>13</v>
+      <c r="B30" s="6">
+        <v>1</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Body Armor'</v>
+        <v>$$Body Armor$$</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="F30" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'Steel-reinforced armor to absord damage from blows and shots.'</v>
+        <v>$$Steel-reinforced armor to absord damage from blows and shots.$$</v>
       </c>
       <c r="G30" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="37" t="s">
-        <v>13</v>
+      <c r="H30" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J30" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Upgrade'</v>
+        <v>$$Upgrade$$</v>
       </c>
       <c r="K30" s="23">
         <v>0</v>
@@ -2901,9 +2875,9 @@
       <c r="Q30" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R30" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Body Armor','Steel-reinforced armor to absord damage from blows and shots.',null,'Upgrade',0,2,null,null,1,null,null),</v>
+      <c r="R30" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Body Armor$$,$$Steel-reinforced armor to absord damage from blows and shots.$$,$$null$$,$$Upgrade$$,0,2,null,null),</v>
       </c>
       <c r="S30" s="29"/>
       <c r="T30" s="29"/>
@@ -2915,36 +2889,36 @@
     </row>
     <row r="31" spans="1:25" ht="30" customHeight="1">
       <c r="A31" s="29"/>
-      <c r="B31" s="6" t="s">
-        <v>13</v>
+      <c r="B31" s="6">
+        <v>1</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Adrenalin Injection'</v>
+        <v>$$Adrenalin Injection$$</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="F31" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'An injection to increase speed and body function temporarily.'</v>
+        <v>$$An injection to increase speed and body function temporarily.$$</v>
       </c>
       <c r="G31" s="47" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="H31" s="47" t="str">
         <f t="shared" si="4"/>
-        <v>'Rush. No cast sickness.'</v>
+        <v>$$Rush. No cast sickness.$$</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J31" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Upgrade'</v>
+        <v>$$Upgrade$$</v>
       </c>
       <c r="K31" s="23">
         <v>1</v>
@@ -2967,9 +2941,9 @@
       <c r="Q31" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R31" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Adrenalin Injection','An injection to increase speed and body function temporarily.','Rush. No cast sickness.','Upgrade',1,1,null,null,1,null,null),</v>
+      <c r="R31" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Adrenalin Injection$$,$$An injection to increase speed and body function temporarily.$$,$$Rush. No cast sickness.$$,$$Upgrade$$,1,1,null,null),</v>
       </c>
       <c r="S31" s="29"/>
       <c r="T31" s="29"/>
@@ -2981,35 +2955,36 @@
     </row>
     <row r="32" spans="1:25" ht="30" customHeight="1">
       <c r="A32" s="29"/>
-      <c r="B32" s="6" t="s">
-        <v>13</v>
+      <c r="B32" s="6">
+        <v>1</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Reinforced Cranial Implants'</v>
+        <v>$$Reinforced Cranial Implants$$</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="F32" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'Offers head protection as well as a slight increase in brain activity.'</v>
+        <v>$$Offers head protection as well as a slight increase in brain activity.$$</v>
       </c>
       <c r="G32" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="37" t="s">
-        <v>13</v>
+      <c r="H32" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J32" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Upgrade'</v>
+        <v>$$Upgrade$$</v>
       </c>
       <c r="K32" s="23">
         <v>1</v>
@@ -3032,9 +3007,9 @@
       <c r="Q32" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R32" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Reinforced Cranial Implants','Offers head protection as well as a slight increase in brain activity.',null,'Upgrade',1,2,null,null,2,null,null),</v>
+      <c r="R32" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Reinforced Cranial Implants$$,$$Offers head protection as well as a slight increase in brain activity.$$,$$null$$,$$Upgrade$$,1,2,null,null),</v>
       </c>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -3046,35 +3021,36 @@
     </row>
     <row r="33" spans="1:25" ht="30" customHeight="1">
       <c r="A33" s="29"/>
-      <c r="B33" s="6" t="s">
-        <v>13</v>
+      <c r="B33" s="6">
+        <v>1</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Steroid Implants'</v>
+        <v>$$Steroid Implants$$</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="F33" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'Intraveneous implants that feed the body for increased strength.'</v>
+        <v>$$Intraveneous implants that feed the body for increased strength.$$</v>
       </c>
       <c r="G33" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="37" t="s">
-        <v>13</v>
+      <c r="H33" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J33" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Upgrade'</v>
+        <v>$$Upgrade$$</v>
       </c>
       <c r="K33" s="23">
         <v>2</v>
@@ -3097,9 +3073,9 @@
       <c r="Q33" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R33" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Steroid Implants','Intraveneous implants that feed the body for increased strength.',null,'Upgrade',2,1,null,null,2,null,null),</v>
+      <c r="R33" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Steroid Implants$$,$$Intraveneous implants that feed the body for increased strength.$$,$$null$$,$$Upgrade$$,2,1,null,null),</v>
       </c>
       <c r="S33" s="29"/>
       <c r="T33" s="29"/>
@@ -3111,36 +3087,36 @@
     </row>
     <row r="34" spans="1:25" ht="30" customHeight="1">
       <c r="A34" s="29"/>
-      <c r="B34" s="6" t="s">
-        <v>13</v>
+      <c r="B34" s="6">
+        <v>1</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Cybernetic Arm Cannon'</v>
+        <v>$$Cybernetic Arm Cannon$$</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="F34" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'Replaces the forearm with a powerful firearm for massive damage.'</v>
+        <v>$$Replaces the forearm with a powerful firearm for massive damage.$$</v>
       </c>
       <c r="G34" s="37" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="H34" s="37" t="str">
         <f t="shared" si="4"/>
-        <v>'Ranged. Suffers no damage when attacking.'</v>
+        <v>$$Ranged. Suffers no damage when attacking.$$</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J34" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Upgrade'</v>
+        <v>$$Upgrade$$</v>
       </c>
       <c r="K34" s="23">
         <v>3</v>
@@ -3163,9 +3139,9 @@
       <c r="Q34" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R34" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Cybernetic Arm Cannon','Replaces the forearm with a powerful firearm for massive damage.','Ranged. Suffers no damage when attacking.','Upgrade',3,0,null,null,2,null,null),</v>
+      <c r="R34" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Cybernetic Arm Cannon$$,$$Replaces the forearm with a powerful firearm for massive damage.$$,$$Ranged. Suffers no damage when attacking.$$,$$Upgrade$$,3,0,null,null),</v>
       </c>
       <c r="S34" s="29"/>
       <c r="T34" s="29"/>
@@ -3177,35 +3153,36 @@
     </row>
     <row r="35" spans="1:25" ht="30" customHeight="1">
       <c r="A35" s="29"/>
-      <c r="B35" s="6" t="s">
-        <v>13</v>
+      <c r="B35" s="6">
+        <v>1</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Exoskeleton'</v>
+        <v>$$Exoskeleton$$</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="F35" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'This very invasive operation reinforces bone tissue with titanium.'</v>
+        <v>$$This very invasive operation reinforces bone tissue with titanium.$$</v>
       </c>
       <c r="G35" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H35" s="37" t="s">
-        <v>13</v>
+      <c r="H35" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J35" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Upgrade'</v>
+        <v>$$Upgrade$$</v>
       </c>
       <c r="K35" s="23">
         <v>0</v>
@@ -3228,9 +3205,9 @@
       <c r="Q35" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R35" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Exoskeleton','This very invasive operation reinforces bone tissue with titanium.',null,'Upgrade',0,3,null,null,2,null,null),</v>
+      <c r="R35" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Exoskeleton$$,$$This very invasive operation reinforces bone tissue with titanium.$$,$$null$$,$$Upgrade$$,0,3,null,null),</v>
       </c>
       <c r="S35" s="29"/>
       <c r="T35" s="29"/>
@@ -3242,35 +3219,36 @@
     </row>
     <row r="36" spans="1:25" ht="42">
       <c r="A36" s="29"/>
-      <c r="B36" s="6" t="s">
-        <v>13</v>
+      <c r="B36" s="6">
+        <v>1</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>'Artificial Intelligence Implants'</v>
+        <v>$$Artificial Intelligence Implants$$</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="F36" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>'An advanced processor is connected to the subject's brain, replacing personality with extreme intelligence and reflexes.'</v>
+        <v>$$An advanced processor is connected to the subject's brain, replacing personality with extreme intelligence and reflexes.$$</v>
       </c>
       <c r="G36" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H36" s="37" t="s">
-        <v>13</v>
+      <c r="H36" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J36" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Upgrade'</v>
+        <v>$$Upgrade$$</v>
       </c>
       <c r="K36" s="23">
         <v>2</v>
@@ -3293,9 +3271,9 @@
       <c r="Q36" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R36" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Artificial Intelligence Implants','An advanced processor is connected to the subject's brain, replacing personality with extreme intelligence and reflexes.',null,'Upgrade',2,2,null,null,3,null,null),</v>
+      <c r="R36" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Artificial Intelligence Implants$$,$$An advanced processor is connected to the subject's brain, replacing personality with extreme intelligence and reflexes.$$,$$null$$,$$Upgrade$$,2,2,null,null),</v>
       </c>
       <c r="S36" s="29"/>
       <c r="T36" s="29"/>
@@ -3306,35 +3284,36 @@
       <c r="Y36" s="29"/>
     </row>
     <row r="37" spans="1:25" s="3" customFormat="1" ht="42">
-      <c r="B37" s="7" t="s">
-        <v>13</v>
+      <c r="B37" s="7">
+        <v>1</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="D37" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>'Full-body Cybernetics'</v>
+        <v>$$Full-body Cybernetics$$</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="F37" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>'Most of the subject's body is converted to cybernetics, increasing strength and resilience substantially.'</v>
+        <v>$$Most of the subject's body is converted to cybernetics, increasing strength and resilience substantially.$$</v>
       </c>
       <c r="G37" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="H37" s="39" t="s">
-        <v>13</v>
+      <c r="H37" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v>$$null$$</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J37" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K37" s="26">
         <v>3</v>
@@ -3357,43 +3336,43 @@
       <c r="Q37" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="R37" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Full-body Cybernetics','Most of the subject's body is converted to cybernetics, increasing strength and resilience substantially.',null,'Spell',3,3,null,null,5,null,null),</v>
+      <c r="R37" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Full-body Cybernetics$$,$$Most of the subject's body is converted to cybernetics, increasing strength and resilience substantially.$$,$$null$$,$$Upgrade$$,3,3,null,null),</v>
       </c>
     </row>
     <row r="38" spans="1:25" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A38" s="29"/>
-      <c r="B38" s="13" t="s">
-        <v>13</v>
+      <c r="B38" s="13">
+        <v>1</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D38" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>'Dumpster'</v>
+        <v>$$Dumpster$$</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F38" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>'It is not unusual to find useful parts in garbage dumpsters in the city.'</v>
+        <v>$$It is not unusual to find useful parts in garbage dumpsters in the city.$$</v>
       </c>
       <c r="G38" s="43" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="H38" s="43" t="str">
         <f t="shared" si="4"/>
-        <v>'Gain 3 Scrap this turn only.'</v>
+        <v>$$Gain 3 Scrap this turn only.$$</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J38" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>13</v>
@@ -3416,9 +3395,9 @@
       <c r="Q38" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R38" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Dumpster','It is not unusual to find useful parts in garbage dumpsters in the city.','Gain 3 Scrap this turn only.','Spell',null,null,3,null,null,null,null),</v>
+      <c r="R38" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Dumpster$$,$$It is not unusual to find useful parts in garbage dumpsters in the city.$$,$$Gain 3 Scrap this turn only.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S38" s="29"/>
       <c r="T38" s="29"/>
@@ -3430,36 +3409,36 @@
     </row>
     <row r="39" spans="1:25" ht="30" customHeight="1">
       <c r="A39" s="29"/>
-      <c r="B39" s="6" t="s">
-        <v>13</v>
+      <c r="B39" s="6">
+        <v>1</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D39" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>'Scrapyard'</v>
+        <v>$$Scrapyard$$</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F39" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>'Raid a scrapyard to find a plethora of useful robotic electronics.'</v>
+        <v>$$Raid a scrapyard to find a plethora of useful robotic electronics.$$</v>
       </c>
       <c r="G39" s="43" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="H39" s="43" t="str">
         <f t="shared" si="4"/>
-        <v>'Gain 5 Scrap this turn only.'</v>
+        <v>$$Gain 5 Scrap this turn only.$$</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J39" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>13</v>
@@ -3482,9 +3461,9 @@
       <c r="Q39" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R39" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Scrapyard','Raid a scrapyard to find a plethora of useful robotic electronics.','Gain 5 Scrap this turn only.','Spell',null,null,5,null,null,null,null),</v>
+      <c r="R39" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Scrapyard$$,$$Raid a scrapyard to find a plethora of useful robotic electronics.$$,$$Gain 5 Scrap this turn only.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S39" s="29"/>
       <c r="T39" s="29"/>
@@ -3496,36 +3475,36 @@
     </row>
     <row r="40" spans="1:25" ht="30" customHeight="1">
       <c r="A40" s="29"/>
-      <c r="B40" s="6" t="s">
-        <v>13</v>
+      <c r="B40" s="6">
+        <v>1</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D40" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'Thievery'</v>
+        <v>$$Thievery$$</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="F40" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'No need to sacrifice your own Mechs now, is there.'</v>
+        <v>$$No need to sacrifice your own Mechs now, is there.$$</v>
       </c>
       <c r="G40" s="44" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="H40" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Steal 3 Scrap from opponent.'</v>
+        <v>$$Steal 3 Scrap from opponent.$$</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J40" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K40" s="11" t="s">
         <v>13</v>
@@ -3548,9 +3527,9 @@
       <c r="Q40" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R40" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Thievery','No need to sacrifice your own Mechs now, is there.','Steal 3 Scrap from opponent.','Spell',null,null,4,null,null,null,null),</v>
+      <c r="R40" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Thievery$$,$$No need to sacrifice your own Mechs now, is there.$$,$$Steal 3 Scrap from opponent.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S40" s="29"/>
       <c r="T40" s="29"/>
@@ -3562,36 +3541,36 @@
     </row>
     <row r="41" spans="1:25" ht="30" customHeight="1">
       <c r="A41" s="29"/>
-      <c r="B41" s="6" t="s">
-        <v>13</v>
+      <c r="B41" s="6">
+        <v>1</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'Pyromania'</v>
+        <v>$$Pyromania$$</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="F41" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'A bottle, a rag, and some fuel; perfect recipe to set a scrap pile ablaze.'</v>
+        <v>$$A bottle, a rag, and some fuel; perfect recipe to set a scrap pile ablaze.$$</v>
       </c>
       <c r="G41" s="44" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="H41" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Opponent loses all Scrap.'</v>
+        <v>$$Opponent loses all Scrap.$$</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J41" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K41" s="11" t="s">
         <v>13</v>
@@ -3614,9 +3593,9 @@
       <c r="Q41" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R41" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Pyromania','A bottle, a rag, and some fuel; perfect recipe to set a scrap pile ablaze.','Opponent loses all Scrap.','Spell',null,null,4,null,null,null,null),</v>
+      <c r="R41" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Pyromania$$,$$A bottle, a rag, and some fuel; perfect recipe to set a scrap pile ablaze.$$,$$Opponent loses all Scrap.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S41" s="29"/>
       <c r="T41" s="29"/>
@@ -3628,36 +3607,36 @@
     </row>
     <row r="42" spans="1:25" ht="30" customHeight="1">
       <c r="A42" s="29"/>
-      <c r="B42" s="6" t="s">
-        <v>13</v>
+      <c r="B42" s="6">
+        <v>1</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="D42" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'EMP'</v>
+        <v>$$EMP$$</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="F42" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'This nuclear device is highly damaging to electronic equipment.'</v>
+        <v>$$This nuclear device is highly damaging to electronic equipment.$$</v>
       </c>
       <c r="G42" s="44" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="H42" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Destroy all Mechs; players gain their Scrap value.'</v>
+        <v>$$Destroy all Mechs; players gain their Scrap value.$$</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J42" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K42" s="11" t="s">
         <v>13</v>
@@ -3680,9 +3659,9 @@
       <c r="Q42" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R42" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('EMP','This nuclear device is highly damaging to electronic equipment.','Destroy all Mechs; players gain their Scrap value.','Spell',null,null,6,null,null,null,null),</v>
+      <c r="R42" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$EMP$$,$$This nuclear device is highly damaging to electronic equipment.$$,$$Destroy all Mechs; players gain their Scrap value.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S42" s="29"/>
       <c r="T42" s="29"/>
@@ -3694,36 +3673,36 @@
     </row>
     <row r="43" spans="1:25" ht="30" customHeight="1">
       <c r="A43" s="29"/>
-      <c r="B43" s="6" t="s">
-        <v>13</v>
+      <c r="B43" s="6">
+        <v>1</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D43" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'Head Shot'</v>
+        <v>$$Head Shot$$</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="F43" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'An accurate shot from a sniper is often enough to take down a person.'</v>
+        <v>$$An accurate shot from a sniper is often enough to take down a person.$$</v>
       </c>
       <c r="G43" s="44" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="H43" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Destroy one Bio unit with 5 Health or less.'</v>
+        <v>$$Destroy one Bio unit with 5 Health or less.$$</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J43" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K43" s="11" t="s">
         <v>13</v>
@@ -3746,9 +3725,9 @@
       <c r="Q43" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R43" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Head Shot','An accurate shot from a sniper is often enough to take down a person.','Destroy one Bio unit with 5 Health or less.','Spell',null,null,4,null,null,null,null),</v>
+      <c r="R43" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Head Shot$$,$$An accurate shot from a sniper is often enough to take down a person.$$,$$Destroy one Bio unit with 5 Health or less.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S43" s="29"/>
       <c r="T43" s="29"/>
@@ -3760,36 +3739,36 @@
     </row>
     <row r="44" spans="1:25" ht="30" customHeight="1">
       <c r="A44" s="29"/>
-      <c r="B44" s="6" t="s">
-        <v>13</v>
+      <c r="B44" s="6">
+        <v>1</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'Immolate'</v>
+        <v>$$Immolate$$</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="F44" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'When bullets are not enough, a massive flame can go a long way.'</v>
+        <v>$$When bullets are not enough, a massive flame can go a long way.$$</v>
       </c>
       <c r="G44" s="44" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="H44" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Destroy one Bio unit with 6 Health or more.'</v>
+        <v>$$Destroy one Bio unit with 6 Health or more.$$</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J44" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K44" s="11" t="s">
         <v>13</v>
@@ -3812,9 +3791,9 @@
       <c r="Q44" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R44" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Immolate','When bullets are not enough, a massive flame can go a long way.','Destroy one Bio unit with 6 Health or more.','Spell',null,null,8,null,null,null,null),</v>
+      <c r="R44" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Immolate$$,$$When bullets are not enough, a massive flame can go a long way.$$,$$Destroy one Bio unit with 6 Health or more.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S44" s="29"/>
       <c r="T44" s="29"/>
@@ -3826,36 +3805,36 @@
     </row>
     <row r="45" spans="1:25" ht="30" customHeight="1">
       <c r="A45" s="29"/>
-      <c r="B45" s="6" t="s">
-        <v>13</v>
+      <c r="B45" s="6">
+        <v>1</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="D45" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'Downgrade'</v>
+        <v>$$Downgrade$$</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="F45" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'Modern warfare relies very heavily on cybernetics. Perhaps too heavily.'</v>
+        <v>$$Modern warfare relies very heavily on cybernetics. Perhaps too heavily.$$</v>
       </c>
       <c r="G45" s="44" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="H45" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Remove all Upgrades from one Bio.'</v>
+        <v>$$Remove all Upgrades from one Bio.$$</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J45" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K45" s="11" t="s">
         <v>13</v>
@@ -3878,9 +3857,9 @@
       <c r="Q45" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R45" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Downgrade','Modern warfare relies very heavily on cybernetics. Perhaps too heavily.','Remove all Upgrades from one Bio.','Spell',null,null,7,null,null,null,null),</v>
+      <c r="R45" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Downgrade$$,$$Modern warfare relies very heavily on cybernetics. Perhaps too heavily.$$,$$Remove all Upgrades from one Bio.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S45" s="29"/>
       <c r="T45" s="29"/>
@@ -3892,36 +3871,36 @@
     </row>
     <row r="46" spans="1:25" ht="30" customHeight="1">
       <c r="A46" s="29"/>
-      <c r="B46" s="6" t="s">
-        <v>13</v>
+      <c r="B46" s="6">
+        <v>1</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D46" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'Spare Parts '</v>
+        <v>$$Spare Parts $$</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="F46" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'A box of robotic parts you forgot you had kept in your warehouse.'</v>
+        <v>$$A box of robotic parts you forgot you had kept in your warehouse.$$</v>
       </c>
       <c r="G46" s="44" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="H46" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'The next Upgrade you play this turn costs 0 Scrap.'</v>
+        <v>$$The next Upgrade you play this turn costs 0 Scrap.$$</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J46" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K46" s="11" t="s">
         <v>13</v>
@@ -3944,9 +3923,9 @@
       <c r="Q46" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R46" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Spare Parts ','A box of robotic parts you forgot you had kept in your warehouse.','The next Upgrade you play this turn costs 0 Scrap.','Spell',null,null,3,null,null,null,null),</v>
+      <c r="R46" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Spare Parts $$,$$A box of robotic parts you forgot you had kept in your warehouse.$$,$$The next Upgrade you play this turn costs 0 Scrap.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S46" s="29"/>
       <c r="T46" s="29"/>
@@ -3958,36 +3937,36 @@
     </row>
     <row r="47" spans="1:25" ht="30" customHeight="1">
       <c r="A47" s="29"/>
-      <c r="B47" s="6" t="s">
-        <v>13</v>
+      <c r="B47" s="6">
+        <v>1</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="D47" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'Firmware Upgrade'</v>
+        <v>$$Firmware Upgrade$$</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="F47" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'A new version of your Cybernetics Operating System is available.'</v>
+        <v>$$A new version of your Cybernetics Operating System is available.$$</v>
       </c>
       <c r="G47" s="44" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="H47" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Upgrade a Bio +2/+2 for a cost in Mana instead of Scrap.'</v>
+        <v>$$Upgrade a Bio +2/+2 for a cost in Mana instead of Scrap.$$</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J47" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K47" s="11">
         <v>2</v>
@@ -4010,9 +3989,9 @@
       <c r="Q47" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R47" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Firmware Upgrade','A new version of your Cybernetics Operating System is available.','Upgrade a Bio +2/+2 for a cost in Mana instead of Scrap.','Spell',2,2,4,null,null,null,null),</v>
+      <c r="R47" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Firmware Upgrade$$,$$A new version of your Cybernetics Operating System is available.$$,$$Upgrade a Bio +2/+2 for a cost in Mana instead of Scrap.$$,$$Spell$$,2,2,null,null),</v>
       </c>
       <c r="S47" s="29"/>
       <c r="T47" s="29"/>
@@ -4024,36 +4003,36 @@
     </row>
     <row r="48" spans="1:25" ht="30" customHeight="1">
       <c r="A48" s="29"/>
-      <c r="B48" s="6" t="s">
-        <v>13</v>
+      <c r="B48" s="6">
+        <v>1</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D48" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'CPU Upgrade '</v>
+        <v>$$CPU Upgrade $$</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="F48" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'Specialized engineers have developed a powerful computer chip. For a price.'</v>
+        <v>$$Specialized engineers have developed a powerful computer chip. For a price.$$</v>
       </c>
       <c r="G48" s="44" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="H48" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Upgrade a Mech +3/+3 for a cost in Scrap.'</v>
+        <v>$$Upgrade a Mech +3/+3 for a cost in Scrap.$$</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J48" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K48" s="11">
         <v>3</v>
@@ -4076,9 +4055,9 @@
       <c r="Q48" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R48" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('CPU Upgrade ','Specialized engineers have developed a powerful computer chip. For a price.','Upgrade a Mech +3/+3 for a cost in Scrap.','Spell',3,3,0,null,3,null,null),</v>
+      <c r="R48" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$CPU Upgrade $$,$$Specialized engineers have developed a powerful computer chip. For a price.$$,$$Upgrade a Mech +3/+3 for a cost in Scrap.$$,$$Spell$$,3,3,null,null),</v>
       </c>
       <c r="S48" s="29"/>
       <c r="T48" s="29"/>
@@ -4090,36 +4069,36 @@
     </row>
     <row r="49" spans="1:25" ht="30" customHeight="1">
       <c r="A49" s="29"/>
-      <c r="B49" s="6" t="s">
-        <v>13</v>
+      <c r="B49" s="6">
+        <v>1</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D49" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'Magnetic Field'</v>
+        <v>$$Magnetic Field$$</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="F49" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'A strong magnetic field to keep all Mechs glued to the battlefield.'</v>
+        <v>$$A strong magnetic field to keep all Mechs glued to the battlefield.$$</v>
       </c>
       <c r="G49" s="44" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="H49" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Opponent cannot scrap Mechs next turn.'</v>
+        <v>$$Opponent cannot scrap Mechs next turn.$$</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J49" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K49" s="11" t="s">
         <v>13</v>
@@ -4142,9 +4121,9 @@
       <c r="Q49" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R49" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Magnetic Field','A strong magnetic field to keep all Mechs glued to the battlefield.','Opponent cannot scrap Mechs next turn.','Spell',null,null,3,null,null,null,null),</v>
+      <c r="R49" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Magnetic Field$$,$$A strong magnetic field to keep all Mechs glued to the battlefield.$$,$$Opponent cannot scrap Mechs next turn.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S49" s="29"/>
       <c r="T49" s="29"/>
@@ -4156,36 +4135,36 @@
     </row>
     <row r="50" spans="1:25" ht="30" customHeight="1">
       <c r="A50" s="29"/>
-      <c r="B50" s="6" t="s">
-        <v>13</v>
+      <c r="B50" s="6">
+        <v>1</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D50" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'Derelict'</v>
+        <v>$$Derelict$$</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="F50" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'Low morale discourages new troops from joining the fight.'</v>
+        <v>$$Low morale discourages new troops from joining the fight.$$</v>
       </c>
       <c r="G50" s="44" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="H50" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Opponent cannot play Bios next turn.'</v>
+        <v>$$Opponent cannot play Bios next turn.$$</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J50" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K50" s="11" t="s">
         <v>13</v>
@@ -4208,9 +4187,9 @@
       <c r="Q50" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R50" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Derelict','Low morale discourages new troops from joining the fight.','Opponent cannot play Bios next turn.','Spell',null,null,3,null,null,null,null),</v>
+      <c r="R50" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Derelict$$,$$Low morale discourages new troops from joining the fight.$$,$$Opponent cannot play Bios next turn.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S50" s="29"/>
       <c r="T50" s="29"/>
@@ -4222,36 +4201,36 @@
     </row>
     <row r="51" spans="1:25" ht="30" customHeight="1">
       <c r="A51" s="29"/>
-      <c r="B51" s="6" t="s">
-        <v>13</v>
+      <c r="B51" s="6">
+        <v>1</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D51" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'Hobble'</v>
+        <v>$$Hobble$$</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="F51" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'Your lead engineer suffered an injury and needs time to heal.'</v>
+        <v>$$Your lead engineer suffered an injury and needs time to heal.$$</v>
       </c>
       <c r="G51" s="44" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="H51" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Opponent cannot play any Upgrade next turn.'</v>
+        <v>$$Opponent cannot play any Upgrade next turn.$$</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J51" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K51" s="11" t="s">
         <v>13</v>
@@ -4274,9 +4253,9 @@
       <c r="Q51" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R51" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Hobble','Your lead engineer suffered an injury and needs time to heal.','Opponent cannot play any Upgrade next turn.','Spell',null,null,3,null,null,null,null),</v>
+      <c r="R51" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Hobble$$,$$Your lead engineer suffered an injury and needs time to heal.$$,$$Opponent cannot play any Upgrade next turn.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S51" s="29"/>
       <c r="T51" s="29"/>
@@ -4288,36 +4267,36 @@
     </row>
     <row r="52" spans="1:25" ht="30" customHeight="1">
       <c r="A52" s="29"/>
-      <c r="B52" s="6" t="s">
-        <v>13</v>
+      <c r="B52" s="6">
+        <v>1</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D52" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'Rust Storm '</v>
+        <v>$$Rust Storm $$</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="F52" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'Corrosion causes armor plates to crack and weaken.'</v>
+        <v>$$Corrosion causes armor plates to crack and weaken.$$</v>
       </c>
       <c r="G52" s="44" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="H52" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Deal 2 damage to all Mechs.'</v>
+        <v>$$Deal 2 damage to all Mechs.$$</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J52" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K52" s="11" t="s">
         <v>13</v>
@@ -4340,9 +4319,9 @@
       <c r="Q52" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R52" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Rust Storm ','Corrosion causes armor plates to crack and weaken.','Deal 2 damage to all Mechs.','Spell',null,null,6,null,null,null,null),</v>
+      <c r="R52" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Rust Storm $$,$$Corrosion causes armor plates to crack and weaken.$$,$$Deal 2 damage to all Mechs.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S52" s="29"/>
       <c r="T52" s="29"/>
@@ -4354,36 +4333,36 @@
     </row>
     <row r="53" spans="1:25" ht="30" customHeight="1">
       <c r="A53" s="29"/>
-      <c r="B53" s="6" t="s">
-        <v>13</v>
+      <c r="B53" s="6">
+        <v>1</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D53" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'Power Surge'</v>
+        <v>$$Power Surge$$</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="F53" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'A surge in the electrical system causes a strange, temporary boost in machines.'</v>
+        <v>$$A surge in the electrical system causes a strange, temporary boost in machines.$$</v>
       </c>
       <c r="G53" s="44" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="H53" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Owned Mechs gain 2 Attack this turn only.'</v>
+        <v>$$Owned Mechs gain 2 Attack this turn only.$$</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J53" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K53" s="11" t="s">
         <v>13</v>
@@ -4406,9 +4385,9 @@
       <c r="Q53" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R53" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Power Surge','A surge in the electrical system causes a strange, temporary boost in machines.','Owned Mechs gain 2 Attack this turn only.','Spell',null,null,4,null,null,null,null),</v>
+      <c r="R53" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Power Surge$$,$$A surge in the electrical system causes a strange, temporary boost in machines.$$,$$Owned Mechs gain 2 Attack this turn only.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S53" s="29"/>
       <c r="T53" s="29"/>
@@ -4420,36 +4399,36 @@
     </row>
     <row r="54" spans="1:25" ht="30" customHeight="1">
       <c r="A54" s="29"/>
-      <c r="B54" s="6" t="s">
-        <v>13</v>
+      <c r="B54" s="6">
+        <v>1</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D54" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>'Heat Shielding '</v>
+        <v>$$Heat Shielding $$</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="F54" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>'Deploy a shield to protect mechanical units for a short time against incoming attacks.'</v>
+        <v>$$Deploy a shield to protect mechanical units for a short time against incoming attacks.$$</v>
       </c>
       <c r="G54" s="44" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="H54" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>'Owned Mechs gain 2 Health during next opponent turn.'</v>
+        <v>$$Owned Mechs gain 2 Health during next opponent turn.$$</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J54" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K54" s="11" t="s">
         <v>13</v>
@@ -4472,9 +4451,9 @@
       <c r="Q54" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R54" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('Heat Shielding ','Deploy a shield to protect mechanical units for a short time against incoming attacks.','Owned Mechs gain 2 Health during next opponent turn.','Spell',null,null,4,null,null,null,null),</v>
+      <c r="R54" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$Heat Shielding $$,$$Deploy a shield to protect mechanical units for a short time against incoming attacks.$$,$$Owned Mechs gain 2 Health during next opponent turn.$$,$$Spell$$,null,null,null,null),</v>
       </c>
       <c r="S54" s="29"/>
       <c r="T54" s="29"/>
@@ -4485,36 +4464,36 @@
       <c r="Y54" s="29"/>
     </row>
     <row r="55" spans="1:25" s="19" customFormat="1" ht="30" customHeight="1">
-      <c r="B55" s="20" t="s">
-        <v>13</v>
+      <c r="B55" s="20">
+        <v>1</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="D55" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>'First Aid Kit'</v>
+        <v>$$First Aid Kit$$</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="F55" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>'Mitigate combat wounds with this assortment of bandages and medicine.'</v>
+        <v>$$Mitigate combat wounds with this assortment of bandages and medicine.$$</v>
       </c>
       <c r="G55" s="38" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="H55" s="38" t="str">
         <f t="shared" si="4"/>
-        <v>'Restore 3 health to the player.'</v>
+        <v>$$Restore 3 health to the player.$$</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J55" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>'Spell'</v>
+        <v>$$Spell$$</v>
       </c>
       <c r="K55" s="22" t="s">
         <v>13</v>
@@ -4537,42 +4516,42 @@
       <c r="Q55" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="R55" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>('First Aid Kit','Mitigate combat wounds with this assortment of bandages and medicine.','Restore 3 health to the player.','Spell',null,null,3,null,null,null,null),</v>
+      <c r="R55" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>(1,$$First Aid Kit$$,$$Mitigate combat wounds with this assortment of bandages and medicine.$$,$$Restore 3 health to the player.$$,$$Spell$$,null,null,null,null),</v>
       </c>
     </row>
     <row r="56" spans="1:25" s="19" customFormat="1" ht="30" customHeight="1">
-      <c r="B56" s="20" t="s">
-        <v>13</v>
+      <c r="B56" s="20">
+        <v>1</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="D56" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>'Emergency Surgery'</v>
+        <v>$$Emergency Surgery$$</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="F56" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>'Expensive surgery to repair broken bones and patch up ripped flesh and muscle.'</v>
+        <v>$$Expensive surgery to repair broken bones and patch up ripped flesh and muscle.$$</v>
       </c>
       <c r="G56" s="38" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="H56" s="38" t="str">
         <f t="shared" si="4"/>
-        <v>'Restore 10 health to the player.'</v>
+        <v>$$Restore 10 health to the player.$$</v>
       </c>
       <c r="I56" s="19" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J56" s="19" t="str">
         <f t="shared" si="2"/>
-        <v>''</v>
+        <v>$$$$</v>
       </c>
       <c r="K56" s="22" t="s">
         <v>13</v>
@@ -4595,19 +4574,17 @@
       <c r="Q56" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="R56" s="11" t="str">
-        <f>"("&amp;D56&amp;","&amp;F56&amp;","&amp;H56&amp;","&amp;J56&amp;","&amp;K56&amp;","&amp;L56&amp;","&amp;M56&amp;","&amp;N56&amp;","&amp;O56&amp;","&amp;P56&amp;","&amp;Q56&amp;");"</f>
-        <v>('Emergency Surgery','Expensive surgery to repair broken bones and patch up ripped flesh and muscle.','Restore 10 health to the player.','',null,null,8,null,null,null,null);</v>
+      <c r="R56" s="23" t="str">
+        <f>"("&amp;B56&amp;",$$"&amp;C56&amp;"$$,$$"&amp;E56&amp;"$$,$$"&amp;G56&amp;"$$,$$"&amp;I56&amp;"$$,"&amp;K56&amp;","&amp;L56&amp;","&amp;P56&amp;","&amp;Q56&amp;"); COMMIT;"</f>
+        <v>(1,$$Emergency Surgery$$,$$Expensive surgery to repair broken bones and patch up ripped flesh and muscle.$$,$$Restore 10 health to the player.$$,$$Spell$$,null,null,null,null); COMMIT;</v>
       </c>
     </row>
     <row r="57" spans="1:25" ht="30" customHeight="1">
-      <c r="R57" s="11" t="str">
-        <f>"COMMIT;"</f>
-        <v>COMMIT;</v>
-      </c>
+      <c r="R57" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated excel and sql files.
</commit_message>
<xml_diff>
--- a/cardshifter-database/TCG card list 10-28-14.xlsx
+++ b/cardshifter-database/TCG card list 10-28-14.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="154">
   <si>
     <t>id</t>
   </si>
@@ -471,9 +471,6 @@
   </si>
   <si>
     <t>Expensive surgery to repair broken bones and patch up ripped flesh and muscle.</t>
-  </si>
-  <si>
-    <t>flavor text</t>
   </si>
   <si>
     <t>Worth more than its weight in scrap, and it is pretty heavy.</t>
@@ -639,8 +636,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -780,7 +785,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -790,6 +795,10 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -799,6 +808,10 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1093,10 +1106,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomLeft" activeCell="R1" sqref="R1:R56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0"/>
@@ -1131,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
@@ -1143,7 +1156,7 @@
         <v>57</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>149</v>
+        <v>57</v>
       </c>
       <c r="G2" s="36" t="s">
         <v>56</v>
@@ -1180,7 +1193,7 @@
       </c>
       <c r="R2" s="23" t="str">
         <f>"START TRANSACTION; SET SEARCH_PATH TO cardshifter_stats; INSERT INTO card("&amp;B2&amp;","&amp;D2&amp;","&amp;F2&amp;","&amp;H2&amp;","&amp;J2&amp;","&amp;K2&amp;","&amp;L2&amp;","&amp;P2&amp;","&amp;Q2&amp;") VALUES"</f>
-        <v>START TRANSACTION; SET SEARCH_PATH TO cardshifter_stats; INSERT INTO card(version,name,flavor text,effect_description,type,attack,health,sickness,attack_available) VALUES</v>
+        <v>START TRANSACTION; SET SEARCH_PATH TO cardshifter_stats; INSERT INTO card(version,name,flavor_text,effect_description,type,attack,health,sickness,attack_available) VALUES</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="30" customHeight="1">
@@ -1295,7 +1308,7 @@
         <v>1</v>
       </c>
       <c r="R4" s="23" t="str">
-        <f t="shared" ref="R4:R55" si="3">"("&amp;B4&amp;",$$"&amp;C4&amp;"$$,$$"&amp;E4&amp;"$$,$$"&amp;G4&amp;"$$,$$"&amp;I4&amp;"$$,"&amp;K4&amp;","&amp;L4&amp;","&amp;P4&amp;","&amp;Q4&amp;"),"</f>
+        <f t="shared" ref="R4:R56" si="3">"("&amp;B4&amp;","&amp;D4&amp;","&amp;F4&amp;","&amp;H4&amp;","&amp;J4&amp;","&amp;K4&amp;","&amp;L4&amp;","&amp;P4&amp;","&amp;Q4&amp;"),"</f>
         <v>(1,$$Gyrodroid$$,$$A flying, spherical droid that shoots weak laser beams at nearby targets.$$,$$Ranged. Suffers no damage when attacking.$$,$$Mech$$,1,1,1,1),</v>
       </c>
     </row>
@@ -1659,7 +1672,7 @@
         <v>$$Supply Mech$$</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F11" s="21" t="str">
         <f t="shared" si="1"/>
@@ -1876,7 +1889,7 @@
       </c>
       <c r="R14" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>(1,$$Waste Runner$$,$$Armored and armed with superior arms.$$,$$null$$,$$Mech$$,4,4,1,1),</v>
+        <v>(1,$$Waste Runner$$,$$Armored and armed with superior arms.$$,$$null$$,$$Hume$$,4,4,1,1),</v>
       </c>
     </row>
     <row r="15" spans="1:18" s="30" customFormat="1" ht="30" customHeight="1">
@@ -2050,7 +2063,7 @@
       </c>
       <c r="R17" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>(1,$$Spook$$,$$Hume that donated their human body to have their consciousness uploaded to the web.$$,$$All friendly Mechs have +1/+1 while this Hume is in play.$$,$$Hume$$,0,5,null,null),</v>
+        <v>(1,$$Spook$$,$$Hume that donated their human body to have their consciousness uploaded to the web.$$,$$All friendly Mechs have +1/+1 while this Hume is in play.$$,$$Bio$$,0,5,null,null),</v>
       </c>
     </row>
     <row r="18" spans="1:25" s="30" customFormat="1" ht="30" customHeight="1">
@@ -2321,7 +2334,7 @@
         <v>$$Field Medic$$</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F22" s="21" t="str">
         <f t="shared" si="1"/>
@@ -2752,7 +2765,7 @@
       </c>
       <c r="R28" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>(1,$$Inside Man$$,$$A government official with wider web control. Usually brings friends.$$,$$Cannot attack. Cast 2 Bodyman minions at no cost next to this unit.$$,$$Bio$$,2,6,1,null),</v>
+        <v>(1,$$Inside Man$$,$$A government official with wider web control. Usually brings friends.$$,$$Cannot attack. Cast 2 Bodyman minions at no cost next to this unit.$$,$$Upgrade$$,2,6,1,null),</v>
       </c>
     </row>
     <row r="29" spans="1:25" s="9" customFormat="1" ht="30" customHeight="1">
@@ -3338,7 +3351,7 @@
       </c>
       <c r="R37" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>(1,$$Full-body Cybernetics$$,$$Most of the subject's body is converted to cybernetics, increasing strength and resilience substantially.$$,$$null$$,$$Upgrade$$,3,3,null,null),</v>
+        <v>(1,$$Full-body Cybernetics$$,$$Most of the subject's body is converted to cybernetics, increasing strength and resilience substantially.$$,$$null$$,$$Spell$$,3,3,null,null),</v>
       </c>
     </row>
     <row r="38" spans="1:25" s="9" customFormat="1" ht="30" customHeight="1">
@@ -4021,7 +4034,7 @@
         <v>$$Specialized engineers have developed a powerful computer chip. For a price.$$</v>
       </c>
       <c r="G48" s="44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H48" s="44" t="str">
         <f t="shared" si="4"/>
@@ -4080,7 +4093,7 @@
         <v>$$Magnetic Field$$</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F49" s="18" t="str">
         <f t="shared" si="1"/>
@@ -4575,8 +4588,8 @@
         <v>13</v>
       </c>
       <c r="R56" s="23" t="str">
-        <f>"("&amp;B56&amp;",$$"&amp;C56&amp;"$$,$$"&amp;E56&amp;"$$,$$"&amp;G56&amp;"$$,$$"&amp;I56&amp;"$$,"&amp;K56&amp;","&amp;L56&amp;","&amp;P56&amp;","&amp;Q56&amp;"); COMMIT;"</f>
-        <v>(1,$$Emergency Surgery$$,$$Expensive surgery to repair broken bones and patch up ripped flesh and muscle.$$,$$Restore 10 health to the player.$$,$$Spell$$,null,null,null,null); COMMIT;</v>
+        <f>"("&amp;B56&amp;","&amp;D56&amp;","&amp;F56&amp;","&amp;H56&amp;","&amp;J56&amp;","&amp;K56&amp;","&amp;L56&amp;","&amp;P56&amp;","&amp;Q56&amp;"); COMMIT;"</f>
+        <v>(1,$$Emergency Surgery$$,$$Expensive surgery to repair broken bones and patch up ripped flesh and muscle.$$,$$Restore 10 health to the player.$$,$$$$,null,null,null,null); COMMIT;</v>
       </c>
     </row>
     <row r="57" spans="1:25" ht="30" customHeight="1">

</xml_diff>